<commit_message>
Mise à jour avec tous les fichiers
</commit_message>
<xml_diff>
--- a/Evaluation.xlsx
+++ b/Evaluation.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Tache</t>
   </si>
@@ -34,17 +34,92 @@
     <t>Christophe TEDALDI</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t xml:space="preserve">Analyse du cahier des charges </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise en place du système de contrôle de version git </t>
+  </si>
+  <si>
+    <t>Mise en commun des travaux de S1</t>
+  </si>
+  <si>
+    <t>Controleur index.php</t>
+  </si>
+  <si>
+    <t>Mise en page avec CSS</t>
+  </si>
+  <si>
+    <t>Affichage des pathologies depuis la base de données</t>
+  </si>
+  <si>
+    <t>Filtrage</t>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
+    <t>Pourcentage de travail</t>
+  </si>
+  <si>
+    <t>Ebauche de l'accueil / Comprehension de Smarty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facilitation acces base de donnée </t>
+  </si>
+  <si>
+    <t>Connexion/Déconnexion utilisateurs</t>
+  </si>
+  <si>
+    <t>Debbugage javascript/classDB</t>
+  </si>
+  <si>
+    <t>Ajout de l'autocompletion</t>
+  </si>
+  <si>
+    <t>Web Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESTE A FAIRE </t>
+  </si>
+  <si>
+    <t>Recherche par mots clés</t>
+  </si>
+  <si>
+    <t>phpDoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pagination qui deconne </t>
+  </si>
+  <si>
+    <t>si on a le temps …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Une page mon compte </t>
+  </si>
+  <si>
+    <t>Total Validator</t>
+  </si>
+  <si>
+    <t>CSS Validator</t>
+  </si>
+  <si>
+    <t>Ameillorations visuelles</t>
+  </si>
+  <si>
+    <t>Web Service</t>
+  </si>
+  <si>
+    <t>Menu + debut doc</t>
+  </si>
+  <si>
+    <t>Documentation + revision index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +130,29 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -78,27 +176,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -114,7 +218,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -400,63 +504,325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="47.08984375" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" style="1" customWidth="1"/>
-    <col min="3" max="7" width="17.6328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.08984375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1">
-        <v>42404</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B25" s="1">
+        <f>SUM(B2:B24)</f>
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" ref="C25:F25" si="0">SUM(C2:C24)</f>
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="4">
+        <f>SUM(B2:B24)/SUM($B2:$F24)</f>
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="C26" s="4">
+        <f t="shared" ref="C26:F26" si="1">SUM(C2:C24)/SUM($B2:$F24)</f>
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" si="1"/>
+        <v>0.49333333333333335</v>
+      </c>
+      <c r="E26" s="4">
+        <f t="shared" si="1"/>
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="F26" s="4">
+        <f t="shared" si="1"/>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="6"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>